<commit_message>
added the functionality of checking for US numbers with area code +1
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,70 +424,196 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>+2348012345678</t>
+          <t>07025664511</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>+2348023456789</t>
+          <t>0702 5664 511</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>+2348034567890</t>
+          <t>0703 331 3456</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>+2348045678901</t>
+          <t>070 3444 2345</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>+2348056789012</t>
+          <t>07125664511</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>+234 806 789 0123</t>
+          <t>0712 5664 511</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>+234 811 234 5678</t>
+          <t>0713 331 3456</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>+234 823 456 7890</t>
+          <t>071 3444 2345</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>+234 824 567 8901</t>
+          <t>08025664511</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>+234 825 678 9012</t>
+          <t>0802 5664 511</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0803 331 3456</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>080 3444 2345</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>08125664511</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0812 5664 511</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>0813 331 3456</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>081 3444 2345</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>09125664511</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>0912 5664 511</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>0913 331 3456</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>091 3444 2345</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>09025664511</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0902 5664 511</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0903 331 3456</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>090 3444 2345</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>+234 445 334 5555</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>+234 445 3344 555</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>+234 4453 345 555</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>+2348123456780</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed the printing loop issue
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,211 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>07025664511</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>0702 5664 511</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>0703 331 3456</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>070 3444 2345</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>07125664511</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>0712 5664 511</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>0713 331 3456</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>071 3444 2345</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>08025664511</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>0802 5664 511</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>0803 331 3456</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>080 3444 2345</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>08125664511</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>0812 5664 511</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>0813 331 3456</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>081 3444 2345</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>09125664511</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>0912 5664 511</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>0913 331 3456</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>091 3444 2345</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>09025664511</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>0902 5664 511</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>0903 331 3456</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>090 3444 2345</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>+234 445 334 5555</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>+234 445 3344 555</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>+234 4453 345 555</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>+2348123456780</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>